<commit_message>
"changes: detect name-email more flexible"
</commit_message>
<xml_diff>
--- a/temp/participants.xlsx
+++ b/temp/participants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8369C6-12A5-43C5-B53C-4B604D2628A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FE44AD-8A0A-4023-915F-32AB22130C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4515" yWindow="630" windowWidth="15375" windowHeight="9885" xr2:uid="{95D8FC80-53E0-41DD-8579-F0AF57D6EFDA}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Mariko Jelek</t>
+    <t>Mohammad Ezzeddin Pratama</t>
   </si>
 </sst>
 </file>
@@ -444,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E6C233D-9C34-49F7-A01E-2D3EB066EE9D}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -456,34 +456,45 @@
     <col min="2" max="2" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2"/>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="C12" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
+    <row r="13" spans="1:4">
+      <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
+    <row r="14" spans="1:4">
+      <c r="C14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="mailto:ezzeddinpratama04@gmail.com" xr:uid="{99759AC8-F6F5-4E0B-B7E5-7FC866EF04EA}"/>
-    <hyperlink ref="B3" r:id="rId2" display="mailto:billiardo985@gmail.com" xr:uid="{2C039B1C-4F13-49D0-9FBD-48FC7E3C4449}"/>
+    <hyperlink ref="D14" r:id="rId1" display="mailto:billiardo985@gmail.com" xr:uid="{875DD37E-5762-4E00-B4CE-6427C6CA0B4F}"/>
+    <hyperlink ref="D13" r:id="rId2" display="mailto:ezzeddinpratama04@gmail.com" xr:uid="{5C763C4E-36FC-4961-8331-B315E668016C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>